<commit_message>
changed N/a to None in era2
</commit_message>
<xml_diff>
--- a/data/era2/yearwiseSlamWinners/yearwiseSlamWinners.xlsx
+++ b/data/era2/yearwiseSlamWinners/yearwiseSlamWinners.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodingProjects\DV\tennistrivia\data\era2\yearwiseSlamWinners\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC54DAFB-605B-46C4-8107-C79D10B2BEFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{212E5B78-03CF-482F-A096-C4235605CABE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7240" yWindow="2840" windowWidth="9190" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,9 +42,6 @@
     <t>Edberg</t>
   </si>
   <si>
-    <t>N/a</t>
-  </si>
-  <si>
     <t>Wilander</t>
   </si>
   <si>
@@ -124,6 +121,9 @@
   </si>
   <si>
     <t>Roddick</t>
+  </si>
+  <si>
+    <t>None</t>
   </si>
 </sst>
 </file>
@@ -443,8 +443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -463,7 +463,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -474,13 +474,13 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
         <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -488,16 +488,16 @@
         <v>1986</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
       <c r="E3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -508,13 +508,13 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -522,16 +522,16 @@
         <v>1988</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D5" t="s">
         <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -539,16 +539,16 @@
         <v>1989</v>
       </c>
       <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
         <v>7</v>
       </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" t="s">
-        <v>8</v>
-      </c>
       <c r="E6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -556,16 +556,16 @@
         <v>1990</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D7" t="s">
         <v>4</v>
       </c>
       <c r="E7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -573,13 +573,13 @@
         <v>1991</v>
       </c>
       <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
         <v>8</v>
       </c>
-      <c r="C8" t="s">
-        <v>9</v>
-      </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E8" t="s">
         <v>4</v>
@@ -590,13 +590,13 @@
         <v>1992</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E9" t="s">
         <v>4</v>
@@ -607,16 +607,16 @@
         <v>1993</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
@@ -624,16 +624,16 @@
         <v>1994</v>
       </c>
       <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" t="s">
         <v>10</v>
-      </c>
-      <c r="C11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -641,16 +641,16 @@
         <v>1995</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -658,16 +658,16 @@
         <v>1996</v>
       </c>
       <c r="B13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
@@ -675,16 +675,16 @@
         <v>1997</v>
       </c>
       <c r="B14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
@@ -692,16 +692,16 @@
         <v>1998</v>
       </c>
       <c r="B15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
@@ -709,16 +709,16 @@
         <v>1999</v>
       </c>
       <c r="B16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" t="s">
         <v>10</v>
-      </c>
-      <c r="E16" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
@@ -726,16 +726,16 @@
         <v>2000</v>
       </c>
       <c r="B17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
@@ -743,16 +743,16 @@
         <v>2001</v>
       </c>
       <c r="B18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D18" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" t="s">
         <v>26</v>
-      </c>
-      <c r="E18" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
@@ -760,16 +760,16 @@
         <v>2002</v>
       </c>
       <c r="B19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
@@ -777,16 +777,16 @@
         <v>2003</v>
       </c>
       <c r="B20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>